<commit_message>
Update Workflow for an Illumina lane planning example v2.xlsx
</commit_message>
<xml_diff>
--- a/mollab_protocols/lab_general/Workflow for an Illumina lane planning example v2.xlsx
+++ b/mollab_protocols/lab_general/Workflow for an Illumina lane planning example v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/maartje_brouwer_nioz_nl/Documents/Documenten/GitHub/OT2/mollab_protocols/lab_general/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{4ECD7E50-0CEC-47D9-A456-BD3F7948DDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DFBF993-0C8D-4016-8F94-0BCAB12FEF7C}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{4ECD7E50-0CEC-47D9-A456-BD3F7948DDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9336C9FB-DACA-4033-9C3F-D8CA6FA5C205}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" firstSheet="5" activeTab="6" xr2:uid="{F055461D-68E6-4A28-B20A-FDBFF2F597CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="6" xr2:uid="{F055461D-68E6-4A28-B20A-FDBFF2F597CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="867">
   <si>
     <t>Strip 1</t>
   </si>
@@ -2742,6 +2742,264 @@
   </si>
   <si>
     <t>sample_10</t>
+  </si>
+  <si>
+    <t>sample_11</t>
+  </si>
+  <si>
+    <t>sample_12</t>
+  </si>
+  <si>
+    <t>sample_13</t>
+  </si>
+  <si>
+    <t>sample_14</t>
+  </si>
+  <si>
+    <t>sample_15</t>
+  </si>
+  <si>
+    <t>sample_16</t>
+  </si>
+  <si>
+    <t>sample_17</t>
+  </si>
+  <si>
+    <t>sample_18</t>
+  </si>
+  <si>
+    <t>sample_19</t>
+  </si>
+  <si>
+    <t>sample_20</t>
+  </si>
+  <si>
+    <t>sample_21</t>
+  </si>
+  <si>
+    <t>sample_22</t>
+  </si>
+  <si>
+    <t>sample_23</t>
+  </si>
+  <si>
+    <t>sample_24</t>
+  </si>
+  <si>
+    <t>sample_25</t>
+  </si>
+  <si>
+    <t>sample_26</t>
+  </si>
+  <si>
+    <t>sample_27</t>
+  </si>
+  <si>
+    <t>sample_28</t>
+  </si>
+  <si>
+    <t>sample_29</t>
+  </si>
+  <si>
+    <t>sample_30</t>
+  </si>
+  <si>
+    <t>sample_31</t>
+  </si>
+  <si>
+    <t>sample_32</t>
+  </si>
+  <si>
+    <t>sample_33</t>
+  </si>
+  <si>
+    <t>sample_34</t>
+  </si>
+  <si>
+    <t>sample_35</t>
+  </si>
+  <si>
+    <t>sample_36</t>
+  </si>
+  <si>
+    <t>sample_37</t>
+  </si>
+  <si>
+    <t>sample_38</t>
+  </si>
+  <si>
+    <t>sample_39</t>
+  </si>
+  <si>
+    <t>sample_40</t>
+  </si>
+  <si>
+    <t>sample_41</t>
+  </si>
+  <si>
+    <t>sample_42</t>
+  </si>
+  <si>
+    <t>sample_43</t>
+  </si>
+  <si>
+    <t>sample_44</t>
+  </si>
+  <si>
+    <t>sample_45</t>
+  </si>
+  <si>
+    <t>sample_46</t>
+  </si>
+  <si>
+    <t>sample_47</t>
+  </si>
+  <si>
+    <t>sample_48</t>
+  </si>
+  <si>
+    <t>sample_49</t>
+  </si>
+  <si>
+    <t>sample_50</t>
+  </si>
+  <si>
+    <t>sample_51</t>
+  </si>
+  <si>
+    <t>sample_52</t>
+  </si>
+  <si>
+    <t>sample_53</t>
+  </si>
+  <si>
+    <t>sample_54</t>
+  </si>
+  <si>
+    <t>sample_55</t>
+  </si>
+  <si>
+    <t>sample_56</t>
+  </si>
+  <si>
+    <t>sample_57</t>
+  </si>
+  <si>
+    <t>sample_58</t>
+  </si>
+  <si>
+    <t>sample_59</t>
+  </si>
+  <si>
+    <t>sample_60</t>
+  </si>
+  <si>
+    <t>sample_61</t>
+  </si>
+  <si>
+    <t>sample_62</t>
+  </si>
+  <si>
+    <t>sample_63</t>
+  </si>
+  <si>
+    <t>sample_64</t>
+  </si>
+  <si>
+    <t>sample_65</t>
+  </si>
+  <si>
+    <t>sample_66</t>
+  </si>
+  <si>
+    <t>sample_67</t>
+  </si>
+  <si>
+    <t>sample_68</t>
+  </si>
+  <si>
+    <t>sample_69</t>
+  </si>
+  <si>
+    <t>sample_70</t>
+  </si>
+  <si>
+    <t>sample_71</t>
+  </si>
+  <si>
+    <t>sample_72</t>
+  </si>
+  <si>
+    <t>sample_73</t>
+  </si>
+  <si>
+    <t>sample_74</t>
+  </si>
+  <si>
+    <t>sample_75</t>
+  </si>
+  <si>
+    <t>sample_76</t>
+  </si>
+  <si>
+    <t>sample_77</t>
+  </si>
+  <si>
+    <t>sample_78</t>
+  </si>
+  <si>
+    <t>sample_79</t>
+  </si>
+  <si>
+    <t>sample_80</t>
+  </si>
+  <si>
+    <t>sample_81</t>
+  </si>
+  <si>
+    <t>sample_82</t>
+  </si>
+  <si>
+    <t>sample_83</t>
+  </si>
+  <si>
+    <t>sample_84</t>
+  </si>
+  <si>
+    <t>sample_85</t>
+  </si>
+  <si>
+    <t>sample_86</t>
+  </si>
+  <si>
+    <t>sample_87</t>
+  </si>
+  <si>
+    <t>sample_88</t>
+  </si>
+  <si>
+    <t>sample_89</t>
+  </si>
+  <si>
+    <t>sample_90</t>
+  </si>
+  <si>
+    <t>sample_91</t>
+  </si>
+  <si>
+    <t>sample_92</t>
+  </si>
+  <si>
+    <t>sample_93</t>
+  </si>
+  <si>
+    <t>sample_94</t>
+  </si>
+  <si>
+    <t>sample_95</t>
+  </si>
+  <si>
+    <t>sample_96</t>
   </si>
 </sst>
 </file>
@@ -3648,15 +3906,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3667,6 +3916,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -7293,18 +7551,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="135" t="s">
         <v>605</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
       <c r="K1" s="52"/>
       <c r="L1" s="62" t="s">
         <v>137</v>
@@ -7319,18 +7577,18 @@
         <v>140</v>
       </c>
       <c r="P1" s="63"/>
-      <c r="R1" s="138" t="s">
+      <c r="R1" s="135" t="s">
         <v>608</v>
       </c>
-      <c r="S1" s="138"/>
-      <c r="T1" s="138"/>
-      <c r="U1" s="138"/>
-      <c r="V1" s="138"/>
-      <c r="W1" s="138"/>
-      <c r="X1" s="138"/>
-      <c r="Y1" s="138"/>
-      <c r="Z1" s="138"/>
-      <c r="AA1" s="138"/>
+      <c r="S1" s="135"/>
+      <c r="T1" s="135"/>
+      <c r="U1" s="135"/>
+      <c r="V1" s="135"/>
+      <c r="W1" s="135"/>
+      <c r="X1" s="135"/>
+      <c r="Y1" s="135"/>
+      <c r="Z1" s="135"/>
+      <c r="AA1" s="135"/>
     </row>
     <row r="2" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
@@ -7356,7 +7614,7 @@
       <c r="O2" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="P2" s="139" t="s">
+      <c r="P2" s="136" t="s">
         <v>29</v>
       </c>
       <c r="R2" s="7"/>
@@ -7371,7 +7629,7 @@
       <c r="AA2" s="7"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="135" t="s">
+      <c r="A3" s="139" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11">
@@ -7412,8 +7670,8 @@
       <c r="O3" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="P3" s="140"/>
-      <c r="R3" s="135" t="s">
+      <c r="P3" s="137"/>
+      <c r="R3" s="139" t="s">
         <v>0</v>
       </c>
       <c r="S3" s="11">
@@ -7443,7 +7701,7 @@
       <c r="AA3" s="13"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="136"/>
+      <c r="A4" s="140"/>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
@@ -7484,8 +7742,8 @@
       <c r="O4" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="P4" s="140"/>
-      <c r="R4" s="136"/>
+      <c r="P4" s="137"/>
+      <c r="R4" s="140"/>
       <c r="S4" s="64" t="s">
         <v>4</v>
       </c>
@@ -7515,7 +7773,7 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="137"/>
+      <c r="A5" s="141"/>
       <c r="B5" s="8" t="s">
         <v>33</v>
       </c>
@@ -7556,8 +7814,8 @@
       <c r="O5" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="P5" s="140"/>
-      <c r="R5" s="137"/>
+      <c r="P5" s="137"/>
+      <c r="R5" s="141"/>
       <c r="S5" s="65" t="s">
         <v>33</v>
       </c>
@@ -7608,7 +7866,7 @@
       <c r="O6" s="56" t="s">
         <v>183</v>
       </c>
-      <c r="P6" s="140"/>
+      <c r="P6" s="137"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -7619,7 +7877,7 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="135" t="s">
+      <c r="A7" s="139" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="11">
@@ -7660,8 +7918,8 @@
       <c r="O7" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="P7" s="140"/>
-      <c r="R7" s="135" t="s">
+      <c r="P7" s="137"/>
+      <c r="R7" s="139" t="s">
         <v>1</v>
       </c>
       <c r="S7" s="11">
@@ -7691,7 +7949,7 @@
       <c r="AA7" s="13"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="136"/>
+      <c r="A8" s="140"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -7732,8 +7990,8 @@
       <c r="O8" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="P8" s="140"/>
-      <c r="R8" s="136"/>
+      <c r="P8" s="137"/>
+      <c r="R8" s="140"/>
       <c r="S8" s="64" t="s">
         <v>4</v>
       </c>
@@ -7763,7 +8021,7 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="137"/>
+      <c r="A9" s="141"/>
       <c r="B9" s="8" t="s">
         <v>41</v>
       </c>
@@ -7804,8 +8062,8 @@
       <c r="O9" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="P9" s="140"/>
-      <c r="R9" s="137"/>
+      <c r="P9" s="137"/>
+      <c r="R9" s="141"/>
       <c r="S9" s="65" t="s">
         <v>33</v>
       </c>
@@ -7856,7 +8114,7 @@
       <c r="O10" s="56" t="s">
         <v>225</v>
       </c>
-      <c r="P10" s="140"/>
+      <c r="P10" s="137"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -7867,7 +8125,7 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="135" t="s">
+      <c r="A11" s="139" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="11">
@@ -7908,8 +8166,8 @@
       <c r="O11" s="56" t="s">
         <v>236</v>
       </c>
-      <c r="P11" s="140"/>
-      <c r="R11" s="135" t="s">
+      <c r="P11" s="137"/>
+      <c r="R11" s="139" t="s">
         <v>2</v>
       </c>
       <c r="S11" s="11">
@@ -7939,7 +8197,7 @@
       <c r="AA11" s="13"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="136"/>
+      <c r="A12" s="140"/>
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
@@ -7980,8 +8238,8 @@
       <c r="O12" s="56" t="s">
         <v>247</v>
       </c>
-      <c r="P12" s="140"/>
-      <c r="R12" s="136"/>
+      <c r="P12" s="137"/>
+      <c r="R12" s="140"/>
       <c r="S12" s="4" t="s">
         <v>12</v>
       </c>
@@ -8011,7 +8269,7 @@
       </c>
     </row>
     <row r="13" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="137"/>
+      <c r="A13" s="141"/>
       <c r="B13" s="8" t="s">
         <v>49</v>
       </c>
@@ -8052,8 +8310,8 @@
       <c r="O13" s="56" t="s">
         <v>258</v>
       </c>
-      <c r="P13" s="140"/>
-      <c r="R13" s="137"/>
+      <c r="P13" s="137"/>
+      <c r="R13" s="141"/>
       <c r="S13" s="8" t="s">
         <v>41</v>
       </c>
@@ -8104,7 +8362,7 @@
       <c r="O14" s="56" t="s">
         <v>269</v>
       </c>
-      <c r="P14" s="140"/>
+      <c r="P14" s="137"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -8115,7 +8373,7 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="135" t="s">
+      <c r="A15" s="139" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="11">
@@ -8156,8 +8414,8 @@
       <c r="O15" s="56" t="s">
         <v>280</v>
       </c>
-      <c r="P15" s="140"/>
-      <c r="R15" s="135" t="s">
+      <c r="P15" s="137"/>
+      <c r="R15" s="139" t="s">
         <v>3</v>
       </c>
       <c r="S15" s="11">
@@ -8187,7 +8445,7 @@
       <c r="AA15" s="13"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="136"/>
+      <c r="A16" s="140"/>
       <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
@@ -8216,8 +8474,8 @@
       <c r="O16" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="P16" s="140"/>
-      <c r="R16" s="136"/>
+      <c r="P16" s="137"/>
+      <c r="R16" s="140"/>
       <c r="S16" s="4" t="s">
         <v>12</v>
       </c>
@@ -8247,7 +8505,7 @@
       </c>
     </row>
     <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="137"/>
+      <c r="A17" s="141"/>
       <c r="B17" s="8" t="s">
         <v>57</v>
       </c>
@@ -8276,8 +8534,8 @@
       <c r="O17" s="56" t="s">
         <v>302</v>
       </c>
-      <c r="P17" s="140"/>
-      <c r="R17" s="137"/>
+      <c r="P17" s="137"/>
+      <c r="R17" s="141"/>
       <c r="S17" s="8" t="s">
         <v>41</v>
       </c>
@@ -8320,7 +8578,7 @@
       <c r="O18" s="56" t="s">
         <v>313</v>
       </c>
-      <c r="P18" s="140"/>
+      <c r="P18" s="137"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K19" s="52"/>
@@ -8336,8 +8594,8 @@
       <c r="O19" s="56" t="s">
         <v>324</v>
       </c>
-      <c r="P19" s="140"/>
-      <c r="R19" s="135" t="s">
+      <c r="P19" s="137"/>
+      <c r="R19" s="139" t="s">
         <v>607</v>
       </c>
       <c r="S19" s="11">
@@ -8367,18 +8625,18 @@
       <c r="AA19" s="13"/>
     </row>
     <row r="20" spans="1:27" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="138" t="s">
+      <c r="A20" s="135" t="s">
         <v>606</v>
       </c>
-      <c r="B20" s="138"/>
-      <c r="C20" s="138"/>
-      <c r="D20" s="138"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="138"/>
-      <c r="H20" s="138"/>
-      <c r="I20" s="138"/>
-      <c r="J20" s="138"/>
+      <c r="B20" s="135"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="135"/>
+      <c r="E20" s="135"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="135"/>
+      <c r="I20" s="135"/>
+      <c r="J20" s="135"/>
       <c r="K20" s="52"/>
       <c r="L20" s="51" t="s">
         <v>333</v>
@@ -8392,8 +8650,8 @@
       <c r="O20" s="56" t="s">
         <v>335</v>
       </c>
-      <c r="P20" s="140"/>
-      <c r="R20" s="136"/>
+      <c r="P20" s="137"/>
+      <c r="R20" s="140"/>
       <c r="S20" s="4" t="s">
         <v>20</v>
       </c>
@@ -8446,8 +8704,8 @@
       <c r="O21" s="56" t="s">
         <v>346</v>
       </c>
-      <c r="P21" s="140"/>
-      <c r="R21" s="137"/>
+      <c r="P21" s="137"/>
+      <c r="R21" s="141"/>
       <c r="S21" s="8" t="s">
         <v>49</v>
       </c>
@@ -8477,7 +8735,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="135" t="s">
+      <c r="A22" s="139" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="11">
@@ -8518,10 +8776,10 @@
       <c r="O22" s="56" t="s">
         <v>357</v>
       </c>
-      <c r="P22" s="140"/>
+      <c r="P22" s="137"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="136"/>
+      <c r="A23" s="140"/>
       <c r="B23" s="4" t="s">
         <v>59</v>
       </c>
@@ -8562,8 +8820,8 @@
       <c r="O23" s="56" t="s">
         <v>368</v>
       </c>
-      <c r="P23" s="140"/>
-      <c r="R23" s="135" t="s">
+      <c r="P23" s="137"/>
+      <c r="R23" s="139" t="s">
         <v>609</v>
       </c>
       <c r="S23" s="11">
@@ -8593,7 +8851,7 @@
       <c r="AA23" s="13"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="137"/>
+      <c r="A24" s="141"/>
       <c r="B24" s="8" t="s">
         <v>83</v>
       </c>
@@ -8634,8 +8892,8 @@
       <c r="O24" s="56" t="s">
         <v>379</v>
       </c>
-      <c r="P24" s="140"/>
-      <c r="R24" s="136"/>
+      <c r="P24" s="137"/>
+      <c r="R24" s="140"/>
       <c r="S24" s="4" t="s">
         <v>20</v>
       </c>
@@ -8686,8 +8944,8 @@
       <c r="O25" s="57" t="s">
         <v>390</v>
       </c>
-      <c r="P25" s="141"/>
-      <c r="R25" s="137"/>
+      <c r="P25" s="138"/>
+      <c r="R25" s="141"/>
       <c r="S25" s="8" t="s">
         <v>49</v>
       </c>
@@ -8717,7 +8975,7 @@
       </c>
     </row>
     <row r="26" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="135" t="s">
+      <c r="A26" s="139" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="11">
@@ -8758,7 +9016,7 @@
       <c r="O26" s="60" t="s">
         <v>401</v>
       </c>
-      <c r="P26" s="139" t="s">
+      <c r="P26" s="136" t="s">
         <v>32</v>
       </c>
       <c r="R26" s="47"/>
@@ -8773,7 +9031,7 @@
       <c r="AA26" s="47"/>
     </row>
     <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="136"/>
+      <c r="A27" s="140"/>
       <c r="B27" s="4" t="s">
         <v>67</v>
       </c>
@@ -8814,8 +9072,8 @@
       <c r="O27" s="56" t="s">
         <v>412</v>
       </c>
-      <c r="P27" s="140"/>
-      <c r="R27" s="135" t="s">
+      <c r="P27" s="137"/>
+      <c r="R27" s="139" t="s">
         <v>610</v>
       </c>
       <c r="S27" s="11">
@@ -8845,7 +9103,7 @@
       <c r="AA27" s="13"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="137"/>
+      <c r="A28" s="141"/>
       <c r="B28" s="8" t="s">
         <v>91</v>
       </c>
@@ -8886,8 +9144,8 @@
       <c r="O28" s="56" t="s">
         <v>423</v>
       </c>
-      <c r="P28" s="140"/>
-      <c r="R28" s="136"/>
+      <c r="P28" s="137"/>
+      <c r="R28" s="140"/>
       <c r="S28" s="4" t="s">
         <v>28</v>
       </c>
@@ -8926,8 +9184,8 @@
       <c r="O29" s="56" t="s">
         <v>434</v>
       </c>
-      <c r="P29" s="140"/>
-      <c r="R29" s="137"/>
+      <c r="P29" s="137"/>
+      <c r="R29" s="141"/>
       <c r="S29" s="8" t="s">
         <v>57</v>
       </c>
@@ -8945,7 +9203,7 @@
       </c>
     </row>
     <row r="30" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="135" t="s">
+      <c r="A30" s="139" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="11">
@@ -8986,7 +9244,7 @@
       <c r="O30" s="56" t="s">
         <v>445</v>
       </c>
-      <c r="P30" s="140"/>
+      <c r="P30" s="137"/>
       <c r="R30" s="47"/>
       <c r="S30" s="47"/>
       <c r="T30" s="47"/>
@@ -8999,7 +9257,7 @@
       <c r="AA30" s="47"/>
     </row>
     <row r="31" spans="1:27" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="136"/>
+      <c r="A31" s="140"/>
       <c r="B31" s="4" t="s">
         <v>75</v>
       </c>
@@ -9040,22 +9298,22 @@
       <c r="O31" s="56" t="s">
         <v>456</v>
       </c>
-      <c r="P31" s="140"/>
-      <c r="R31" s="138" t="s">
+      <c r="P31" s="137"/>
+      <c r="R31" s="135" t="s">
         <v>611</v>
       </c>
-      <c r="S31" s="138"/>
-      <c r="T31" s="138"/>
-      <c r="U31" s="138"/>
-      <c r="V31" s="138"/>
-      <c r="W31" s="138"/>
-      <c r="X31" s="138"/>
-      <c r="Y31" s="138"/>
-      <c r="Z31" s="138"/>
-      <c r="AA31" s="138"/>
+      <c r="S31" s="135"/>
+      <c r="T31" s="135"/>
+      <c r="U31" s="135"/>
+      <c r="V31" s="135"/>
+      <c r="W31" s="135"/>
+      <c r="X31" s="135"/>
+      <c r="Y31" s="135"/>
+      <c r="Z31" s="135"/>
+      <c r="AA31" s="135"/>
     </row>
     <row r="32" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="137"/>
+      <c r="A32" s="141"/>
       <c r="B32" s="8" t="s">
         <v>99</v>
       </c>
@@ -9096,7 +9354,7 @@
       <c r="O32" s="56" t="s">
         <v>467</v>
       </c>
-      <c r="P32" s="140"/>
+      <c r="P32" s="137"/>
       <c r="R32" s="7"/>
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
@@ -9130,8 +9388,8 @@
       <c r="O33" s="56" t="s">
         <v>478</v>
       </c>
-      <c r="P33" s="140"/>
-      <c r="R33" s="135" t="s">
+      <c r="P33" s="137"/>
+      <c r="R33" s="139" t="s">
         <v>0</v>
       </c>
       <c r="S33" s="11">
@@ -9161,7 +9419,7 @@
       <c r="AA33" s="13"/>
     </row>
     <row r="34" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="135" t="s">
+      <c r="A34" s="139" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="11">
@@ -9202,8 +9460,8 @@
       <c r="O34" s="56" t="s">
         <v>489</v>
       </c>
-      <c r="P34" s="140"/>
-      <c r="R34" s="136"/>
+      <c r="P34" s="137"/>
+      <c r="R34" s="140"/>
       <c r="S34" s="68" t="s">
         <v>59</v>
       </c>
@@ -9233,7 +9491,7 @@
       </c>
     </row>
     <row r="35" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="136"/>
+      <c r="A35" s="140"/>
       <c r="B35" s="4" t="s">
         <v>107</v>
       </c>
@@ -9262,8 +9520,8 @@
       <c r="O35" s="56" t="s">
         <v>500</v>
       </c>
-      <c r="P35" s="140"/>
-      <c r="R35" s="137"/>
+      <c r="P35" s="137"/>
+      <c r="R35" s="141"/>
       <c r="S35" s="69" t="s">
         <v>83</v>
       </c>
@@ -9293,7 +9551,7 @@
       </c>
     </row>
     <row r="36" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="137"/>
+      <c r="A36" s="141"/>
       <c r="B36" s="8" t="s">
         <v>57</v>
       </c>
@@ -9322,7 +9580,7 @@
       <c r="O36" s="56" t="s">
         <v>509</v>
       </c>
-      <c r="P36" s="140"/>
+      <c r="P36" s="137"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
@@ -9346,8 +9604,8 @@
       <c r="O37" s="56" t="s">
         <v>518</v>
       </c>
-      <c r="P37" s="140"/>
-      <c r="R37" s="135" t="s">
+      <c r="P37" s="137"/>
+      <c r="R37" s="139" t="s">
         <v>1</v>
       </c>
       <c r="S37" s="11">
@@ -9390,8 +9648,8 @@
       <c r="O38" s="56" t="s">
         <v>527</v>
       </c>
-      <c r="P38" s="140"/>
-      <c r="R38" s="136"/>
+      <c r="P38" s="137"/>
+      <c r="R38" s="140"/>
       <c r="S38" s="68" t="s">
         <v>59</v>
       </c>
@@ -9434,8 +9692,8 @@
       <c r="O39" s="56" t="s">
         <v>536</v>
       </c>
-      <c r="P39" s="140"/>
-      <c r="R39" s="137"/>
+      <c r="P39" s="137"/>
+      <c r="R39" s="141"/>
       <c r="S39" s="69" t="s">
         <v>83</v>
       </c>
@@ -9478,7 +9736,7 @@
       <c r="O40" s="56" t="s">
         <v>545</v>
       </c>
-      <c r="P40" s="140"/>
+      <c r="P40" s="137"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
@@ -9502,8 +9760,8 @@
       <c r="O41" s="56" t="s">
         <v>554</v>
       </c>
-      <c r="P41" s="140"/>
-      <c r="R41" s="135" t="s">
+      <c r="P41" s="137"/>
+      <c r="R41" s="139" t="s">
         <v>2</v>
       </c>
       <c r="S41" s="11">
@@ -9546,8 +9804,8 @@
       <c r="O42" s="56" t="s">
         <v>563</v>
       </c>
-      <c r="P42" s="140"/>
-      <c r="R42" s="136"/>
+      <c r="P42" s="137"/>
+      <c r="R42" s="140"/>
       <c r="S42" s="68" t="s">
         <v>67</v>
       </c>
@@ -9590,8 +9848,8 @@
       <c r="O43" s="56" t="s">
         <v>572</v>
       </c>
-      <c r="P43" s="140"/>
-      <c r="R43" s="137"/>
+      <c r="P43" s="137"/>
+      <c r="R43" s="141"/>
       <c r="S43" s="69" t="s">
         <v>91</v>
       </c>
@@ -9634,7 +9892,7 @@
       <c r="O44" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="P44" s="140"/>
+      <c r="P44" s="137"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
@@ -9658,8 +9916,8 @@
       <c r="O45" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="P45" s="140"/>
-      <c r="R45" s="135" t="s">
+      <c r="P45" s="137"/>
+      <c r="R45" s="139" t="s">
         <v>3</v>
       </c>
       <c r="S45" s="11">
@@ -9702,8 +9960,8 @@
       <c r="O46" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="P46" s="140"/>
-      <c r="R46" s="136"/>
+      <c r="P46" s="137"/>
+      <c r="R46" s="140"/>
       <c r="S46" s="68" t="s">
         <v>67</v>
       </c>
@@ -9746,8 +10004,8 @@
       <c r="O47" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="P47" s="140"/>
-      <c r="R47" s="137"/>
+      <c r="P47" s="137"/>
+      <c r="R47" s="141"/>
       <c r="S47" s="69" t="s">
         <v>91</v>
       </c>
@@ -9790,7 +10048,7 @@
       <c r="O48" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="P48" s="140"/>
+      <c r="P48" s="137"/>
     </row>
     <row r="49" spans="11:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K49" s="52"/>
@@ -9806,8 +10064,8 @@
       <c r="O49" s="57" t="s">
         <v>196</v>
       </c>
-      <c r="P49" s="141"/>
-      <c r="R49" s="135" t="s">
+      <c r="P49" s="138"/>
+      <c r="R49" s="139" t="s">
         <v>607</v>
       </c>
       <c r="S49" s="11">
@@ -9837,7 +10095,7 @@
       <c r="AA49" s="13"/>
     </row>
     <row r="50" spans="11:27" x14ac:dyDescent="0.25">
-      <c r="R50" s="136"/>
+      <c r="R50" s="140"/>
       <c r="S50" s="68" t="s">
         <v>75</v>
       </c>
@@ -9867,7 +10125,7 @@
       </c>
     </row>
     <row r="51" spans="11:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R51" s="137"/>
+      <c r="R51" s="141"/>
       <c r="S51" s="69" t="s">
         <v>99</v>
       </c>
@@ -9898,7 +10156,7 @@
     </row>
     <row r="52" spans="11:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="11:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R53" s="135" t="s">
+      <c r="R53" s="139" t="s">
         <v>609</v>
       </c>
       <c r="S53" s="11">
@@ -9928,7 +10186,7 @@
       <c r="AA53" s="13"/>
     </row>
     <row r="54" spans="11:27" x14ac:dyDescent="0.25">
-      <c r="R54" s="136"/>
+      <c r="R54" s="140"/>
       <c r="S54" s="68" t="s">
         <v>75</v>
       </c>
@@ -9958,7 +10216,7 @@
       </c>
     </row>
     <row r="55" spans="11:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R55" s="137"/>
+      <c r="R55" s="141"/>
       <c r="S55" s="69" t="s">
         <v>99</v>
       </c>
@@ -10000,7 +10258,7 @@
       <c r="AA56" s="47"/>
     </row>
     <row r="57" spans="11:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R57" s="135" t="s">
+      <c r="R57" s="139" t="s">
         <v>610</v>
       </c>
       <c r="S57" s="11">
@@ -10030,7 +10288,7 @@
       <c r="AA57" s="13"/>
     </row>
     <row r="58" spans="11:27" x14ac:dyDescent="0.25">
-      <c r="R58" s="136"/>
+      <c r="R58" s="140"/>
       <c r="S58" s="4" t="s">
         <v>107</v>
       </c>
@@ -10048,7 +10306,7 @@
       </c>
     </row>
     <row r="59" spans="11:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R59" s="137"/>
+      <c r="R59" s="141"/>
       <c r="S59" s="8" t="s">
         <v>57</v>
       </c>
@@ -10067,6 +10325,22 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="R49:R51"/>
+    <mergeCell ref="R53:R55"/>
+    <mergeCell ref="R57:R59"/>
+    <mergeCell ref="R41:R43"/>
+    <mergeCell ref="R23:R25"/>
+    <mergeCell ref="R27:R29"/>
+    <mergeCell ref="R31:AA31"/>
+    <mergeCell ref="R45:R47"/>
+    <mergeCell ref="R19:R21"/>
+    <mergeCell ref="R33:R35"/>
+    <mergeCell ref="R37:R39"/>
+    <mergeCell ref="R1:AA1"/>
+    <mergeCell ref="R3:R5"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R15:R17"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="P2:P25"/>
     <mergeCell ref="P26:P49"/>
@@ -10079,22 +10353,6 @@
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A15:A17"/>
-    <mergeCell ref="R19:R21"/>
-    <mergeCell ref="R33:R35"/>
-    <mergeCell ref="R37:R39"/>
-    <mergeCell ref="R1:AA1"/>
-    <mergeCell ref="R3:R5"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="R49:R51"/>
-    <mergeCell ref="R53:R55"/>
-    <mergeCell ref="R57:R59"/>
-    <mergeCell ref="R41:R43"/>
-    <mergeCell ref="R23:R25"/>
-    <mergeCell ref="R27:R29"/>
-    <mergeCell ref="R31:AA31"/>
-    <mergeCell ref="R45:R47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14160,8 +14418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB84F64-FB97-431A-973F-C63A0FB73C6D}">
   <dimension ref="A1:L123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="N98" sqref="N98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14418,17 +14676,21 @@
       <c r="A12" s="129">
         <v>11</v>
       </c>
-      <c r="B12" s="128"/>
+      <c r="B12" s="128" t="s">
+        <v>781</v>
+      </c>
       <c r="C12" s="128"/>
       <c r="D12" s="128"/>
-      <c r="E12" s="128"/>
-      <c r="F12" s="106" t="e">
+      <c r="E12" s="128">
+        <v>90</v>
+      </c>
+      <c r="F12" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G12" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G12" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="I12" s="100"/>
     </row>
@@ -14436,1445 +14698,1785 @@
       <c r="A13" s="129">
         <v>12</v>
       </c>
-      <c r="B13" s="128"/>
+      <c r="B13" s="128" t="s">
+        <v>782</v>
+      </c>
       <c r="C13" s="128"/>
       <c r="D13" s="128"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="106" t="e">
+      <c r="E13" s="128">
+        <v>3</v>
+      </c>
+      <c r="F13" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G13" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G13" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="129">
         <v>13</v>
       </c>
-      <c r="B14" s="128"/>
+      <c r="B14" s="128" t="s">
+        <v>783</v>
+      </c>
       <c r="C14" s="128"/>
       <c r="D14" s="128"/>
-      <c r="E14" s="128"/>
-      <c r="F14" s="106" t="e">
+      <c r="E14" s="128">
+        <v>50</v>
+      </c>
+      <c r="F14" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G14" s="106" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="G14" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="129">
         <v>14</v>
       </c>
-      <c r="B15" s="128"/>
+      <c r="B15" s="128" t="s">
+        <v>784</v>
+      </c>
       <c r="C15" s="128"/>
       <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
-      <c r="F15" s="106" t="e">
+      <c r="E15" s="128">
+        <v>150</v>
+      </c>
+      <c r="F15" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" s="106" t="e">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="G15" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="129">
         <v>15</v>
       </c>
-      <c r="B16" s="128"/>
+      <c r="B16" s="128" t="s">
+        <v>785</v>
+      </c>
       <c r="C16" s="128"/>
       <c r="D16" s="128"/>
-      <c r="E16" s="128"/>
-      <c r="F16" s="106" t="e">
+      <c r="E16" s="128">
+        <v>36</v>
+      </c>
+      <c r="F16" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G16" s="106" t="e">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="G16" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="129">
         <v>16</v>
       </c>
-      <c r="B17" s="128"/>
+      <c r="B17" s="128" t="s">
+        <v>786</v>
+      </c>
       <c r="C17" s="128"/>
       <c r="D17" s="128"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="106" t="e">
+      <c r="E17" s="128">
+        <v>95</v>
+      </c>
+      <c r="F17" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="106" t="e">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="G17" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.42105263157894735</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="129">
         <v>17</v>
       </c>
-      <c r="B18" s="128"/>
+      <c r="B18" s="128" t="s">
+        <v>787</v>
+      </c>
       <c r="C18" s="128"/>
       <c r="D18" s="128"/>
-      <c r="E18" s="128"/>
-      <c r="F18" s="106" t="e">
+      <c r="E18" s="128">
+        <v>5</v>
+      </c>
+      <c r="F18" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G18" s="106" t="e">
+        <v>8</v>
+      </c>
+      <c r="G18" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="129">
         <v>18</v>
       </c>
-      <c r="B19" s="128"/>
+      <c r="B19" s="128" t="s">
+        <v>788</v>
+      </c>
       <c r="C19" s="128"/>
       <c r="D19" s="128"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="106" t="e">
+      <c r="E19" s="128">
+        <v>1.3</v>
+      </c>
+      <c r="F19" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G19" s="106" t="e">
+        <v>30.769230769230766</v>
+      </c>
+      <c r="G19" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>30.769230769230766</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="129">
         <v>19</v>
       </c>
-      <c r="B20" s="128"/>
+      <c r="B20" s="128" t="s">
+        <v>789</v>
+      </c>
       <c r="C20" s="128"/>
       <c r="D20" s="128"/>
-      <c r="E20" s="128"/>
-      <c r="F20" s="106" t="e">
+      <c r="E20" s="128">
+        <v>90</v>
+      </c>
+      <c r="F20" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G20" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G20" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="129">
         <v>20</v>
       </c>
-      <c r="B21" s="128"/>
+      <c r="B21" s="128" t="s">
+        <v>790</v>
+      </c>
       <c r="C21" s="128"/>
       <c r="D21" s="128"/>
-      <c r="E21" s="128"/>
-      <c r="F21" s="106" t="e">
+      <c r="E21" s="128">
+        <v>40</v>
+      </c>
+      <c r="F21" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G21" s="106" t="e">
+        <v>1</v>
+      </c>
+      <c r="G21" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="129">
         <v>21</v>
       </c>
-      <c r="B22" s="128"/>
+      <c r="B22" s="128" t="s">
+        <v>791</v>
+      </c>
       <c r="C22" s="128"/>
       <c r="D22" s="128"/>
-      <c r="E22" s="128"/>
-      <c r="F22" s="106" t="e">
+      <c r="E22" s="128">
+        <v>9</v>
+      </c>
+      <c r="F22" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G22" s="106" t="e">
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="G22" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="129">
         <v>22</v>
       </c>
-      <c r="B23" s="128"/>
+      <c r="B23" s="128" t="s">
+        <v>792</v>
+      </c>
       <c r="C23" s="128"/>
       <c r="D23" s="128"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="106" t="e">
+      <c r="E23" s="128">
+        <v>3</v>
+      </c>
+      <c r="F23" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G23" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G23" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="129">
         <v>23</v>
       </c>
-      <c r="B24" s="128"/>
+      <c r="B24" s="128" t="s">
+        <v>793</v>
+      </c>
       <c r="C24" s="128"/>
       <c r="D24" s="128"/>
-      <c r="E24" s="128"/>
-      <c r="F24" s="106" t="e">
+      <c r="E24" s="128">
+        <v>90</v>
+      </c>
+      <c r="F24" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G24" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G24" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="129">
         <v>24</v>
       </c>
-      <c r="B25" s="128"/>
+      <c r="B25" s="128" t="s">
+        <v>794</v>
+      </c>
       <c r="C25" s="128"/>
       <c r="D25" s="128"/>
-      <c r="E25" s="128"/>
-      <c r="F25" s="106" t="e">
+      <c r="E25" s="128">
+        <v>3</v>
+      </c>
+      <c r="F25" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G25" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G25" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="129">
         <v>25</v>
       </c>
-      <c r="B26" s="128"/>
+      <c r="B26" s="128" t="s">
+        <v>795</v>
+      </c>
       <c r="C26" s="128"/>
       <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="106" t="e">
+      <c r="E26" s="128">
+        <v>1.3</v>
+      </c>
+      <c r="F26" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G26" s="106" t="e">
+        <v>30.769230769230766</v>
+      </c>
+      <c r="G26" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>30.769230769230766</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="129">
         <v>26</v>
       </c>
-      <c r="B27" s="128"/>
+      <c r="B27" s="128" t="s">
+        <v>796</v>
+      </c>
       <c r="C27" s="128"/>
       <c r="D27" s="128"/>
-      <c r="E27" s="128"/>
-      <c r="F27" s="106" t="e">
+      <c r="E27" s="128">
+        <v>90</v>
+      </c>
+      <c r="F27" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G27" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G27" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="129">
         <v>27</v>
       </c>
-      <c r="B28" s="128"/>
+      <c r="B28" s="128" t="s">
+        <v>797</v>
+      </c>
       <c r="C28" s="128"/>
       <c r="D28" s="128"/>
-      <c r="E28" s="128"/>
-      <c r="F28" s="106" t="e">
+      <c r="E28" s="128">
+        <v>40</v>
+      </c>
+      <c r="F28" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G28" s="106" t="e">
+        <v>1</v>
+      </c>
+      <c r="G28" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="129">
         <v>28</v>
       </c>
-      <c r="B29" s="128"/>
+      <c r="B29" s="128" t="s">
+        <v>798</v>
+      </c>
       <c r="C29" s="128"/>
       <c r="D29" s="128"/>
-      <c r="E29" s="128"/>
-      <c r="F29" s="106" t="e">
+      <c r="E29" s="128">
+        <v>9</v>
+      </c>
+      <c r="F29" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G29" s="106" t="e">
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="G29" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="129">
         <v>29</v>
       </c>
-      <c r="B30" s="128"/>
+      <c r="B30" s="128" t="s">
+        <v>799</v>
+      </c>
       <c r="C30" s="128"/>
       <c r="D30" s="128"/>
-      <c r="E30" s="128"/>
-      <c r="F30" s="106" t="e">
+      <c r="E30" s="128">
+        <v>3</v>
+      </c>
+      <c r="F30" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G30" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G30" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="129">
         <v>30</v>
       </c>
-      <c r="B31" s="128"/>
+      <c r="B31" s="128" t="s">
+        <v>800</v>
+      </c>
       <c r="C31" s="128"/>
       <c r="D31" s="128"/>
-      <c r="E31" s="128"/>
-      <c r="F31" s="106" t="e">
+      <c r="E31" s="128">
+        <v>90</v>
+      </c>
+      <c r="F31" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G31" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G31" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="129">
         <v>31</v>
       </c>
-      <c r="B32" s="128"/>
+      <c r="B32" s="128" t="s">
+        <v>801</v>
+      </c>
       <c r="C32" s="128"/>
       <c r="D32" s="128"/>
-      <c r="E32" s="128"/>
-      <c r="F32" s="106" t="e">
+      <c r="E32" s="128">
+        <v>3</v>
+      </c>
+      <c r="F32" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G32" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G32" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="129">
         <v>32</v>
       </c>
-      <c r="B33" s="128"/>
+      <c r="B33" s="128" t="s">
+        <v>802</v>
+      </c>
       <c r="C33" s="128"/>
       <c r="D33" s="128"/>
-      <c r="E33" s="128"/>
-      <c r="F33" s="106" t="e">
+      <c r="E33" s="128">
+        <v>50</v>
+      </c>
+      <c r="F33" s="106">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G33" s="106" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="G33" s="106">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="129">
         <v>33</v>
       </c>
-      <c r="B34" s="128"/>
+      <c r="B34" s="128" t="s">
+        <v>803</v>
+      </c>
       <c r="C34" s="128"/>
       <c r="D34" s="128"/>
-      <c r="E34" s="128"/>
-      <c r="F34" s="106" t="e">
+      <c r="E34" s="128">
+        <v>150</v>
+      </c>
+      <c r="F34" s="106">
         <f t="shared" ref="F34:F65" si="2">40/E34</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G34" s="106" t="e">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="G34" s="106">
         <f t="shared" ref="G34:G65" si="3">IF(E34&lt;0,150,F34)</f>
-        <v>#DIV/0!</v>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="129">
         <v>34</v>
       </c>
-      <c r="B35" s="128"/>
+      <c r="B35" s="128" t="s">
+        <v>804</v>
+      </c>
       <c r="C35" s="128"/>
       <c r="D35" s="128"/>
-      <c r="E35" s="128"/>
-      <c r="F35" s="106" t="e">
+      <c r="E35" s="128">
+        <v>36</v>
+      </c>
+      <c r="F35" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G35" s="106" t="e">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="G35" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="129">
         <v>35</v>
       </c>
-      <c r="B36" s="128"/>
+      <c r="B36" s="128" t="s">
+        <v>805</v>
+      </c>
       <c r="C36" s="128"/>
       <c r="D36" s="128"/>
-      <c r="E36" s="128"/>
-      <c r="F36" s="106" t="e">
+      <c r="E36" s="128">
+        <v>95</v>
+      </c>
+      <c r="F36" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G36" s="106" t="e">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="G36" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.42105263157894735</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="129">
         <v>36</v>
       </c>
-      <c r="B37" s="128"/>
+      <c r="B37" s="128" t="s">
+        <v>806</v>
+      </c>
       <c r="C37" s="128"/>
       <c r="D37" s="128"/>
-      <c r="E37" s="128"/>
-      <c r="F37" s="106" t="e">
+      <c r="E37" s="128">
+        <v>5</v>
+      </c>
+      <c r="F37" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G37" s="106" t="e">
+        <v>8</v>
+      </c>
+      <c r="G37" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="129">
         <v>37</v>
       </c>
-      <c r="B38" s="128"/>
+      <c r="B38" s="128" t="s">
+        <v>807</v>
+      </c>
       <c r="C38" s="128"/>
       <c r="D38" s="128"/>
-      <c r="E38" s="128"/>
-      <c r="F38" s="106" t="e">
+      <c r="E38" s="128">
+        <v>1.3</v>
+      </c>
+      <c r="F38" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G38" s="106" t="e">
+        <v>30.769230769230766</v>
+      </c>
+      <c r="G38" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>30.769230769230766</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="129">
         <v>38</v>
       </c>
-      <c r="B39" s="128"/>
+      <c r="B39" s="128" t="s">
+        <v>808</v>
+      </c>
       <c r="C39" s="128"/>
       <c r="D39" s="128"/>
-      <c r="E39" s="128"/>
-      <c r="F39" s="106" t="e">
+      <c r="E39" s="128">
+        <v>90</v>
+      </c>
+      <c r="F39" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G39" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G39" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="129">
         <v>39</v>
       </c>
-      <c r="B40" s="128"/>
+      <c r="B40" s="128" t="s">
+        <v>809</v>
+      </c>
       <c r="C40" s="128"/>
       <c r="D40" s="128"/>
-      <c r="E40" s="128"/>
-      <c r="F40" s="106" t="e">
+      <c r="E40" s="128">
+        <v>40</v>
+      </c>
+      <c r="F40" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G40" s="106" t="e">
+        <v>1</v>
+      </c>
+      <c r="G40" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="129">
         <v>40</v>
       </c>
-      <c r="B41" s="128"/>
+      <c r="B41" s="128" t="s">
+        <v>810</v>
+      </c>
       <c r="C41" s="128"/>
       <c r="D41" s="128"/>
-      <c r="E41" s="128"/>
-      <c r="F41" s="106" t="e">
+      <c r="E41" s="128">
+        <v>9</v>
+      </c>
+      <c r="F41" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G41" s="106" t="e">
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="G41" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="129">
         <v>41</v>
       </c>
-      <c r="B42" s="128"/>
+      <c r="B42" s="128" t="s">
+        <v>811</v>
+      </c>
       <c r="C42" s="128"/>
       <c r="D42" s="128"/>
-      <c r="E42" s="128"/>
-      <c r="F42" s="106" t="e">
+      <c r="E42" s="128">
+        <v>40</v>
+      </c>
+      <c r="F42" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G42" s="106" t="e">
+        <v>1</v>
+      </c>
+      <c r="G42" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="129">
         <v>42</v>
       </c>
-      <c r="B43" s="128"/>
+      <c r="B43" s="128" t="s">
+        <v>812</v>
+      </c>
       <c r="C43" s="128"/>
       <c r="D43" s="128"/>
-      <c r="E43" s="128"/>
-      <c r="F43" s="106" t="e">
+      <c r="E43" s="128">
+        <v>9</v>
+      </c>
+      <c r="F43" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G43" s="106" t="e">
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="G43" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="129">
         <v>43</v>
       </c>
-      <c r="B44" s="128"/>
+      <c r="B44" s="128" t="s">
+        <v>813</v>
+      </c>
       <c r="C44" s="128"/>
       <c r="D44" s="128"/>
-      <c r="E44" s="128"/>
-      <c r="F44" s="106" t="e">
+      <c r="E44" s="128">
+        <v>3</v>
+      </c>
+      <c r="F44" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G44" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G44" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="129">
         <v>44</v>
       </c>
-      <c r="B45" s="128"/>
+      <c r="B45" s="128" t="s">
+        <v>814</v>
+      </c>
       <c r="C45" s="128"/>
       <c r="D45" s="128"/>
-      <c r="E45" s="128"/>
-      <c r="F45" s="106" t="e">
+      <c r="E45" s="128">
+        <v>90</v>
+      </c>
+      <c r="F45" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G45" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G45" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="129">
         <v>45</v>
       </c>
-      <c r="B46" s="128"/>
+      <c r="B46" s="128" t="s">
+        <v>815</v>
+      </c>
       <c r="C46" s="128"/>
       <c r="D46" s="128"/>
-      <c r="E46" s="128"/>
-      <c r="F46" s="106" t="e">
+      <c r="E46" s="128">
+        <v>3</v>
+      </c>
+      <c r="F46" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G46" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G46" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="129">
         <v>46</v>
       </c>
-      <c r="B47" s="128"/>
+      <c r="B47" s="128" t="s">
+        <v>816</v>
+      </c>
       <c r="C47" s="128"/>
       <c r="D47" s="128"/>
-      <c r="E47" s="128"/>
-      <c r="F47" s="106" t="e">
+      <c r="E47" s="128">
+        <v>50</v>
+      </c>
+      <c r="F47" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G47" s="106" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="G47" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="129">
         <v>47</v>
       </c>
-      <c r="B48" s="128"/>
+      <c r="B48" s="128" t="s">
+        <v>817</v>
+      </c>
       <c r="C48" s="128"/>
       <c r="D48" s="128"/>
-      <c r="E48" s="128"/>
-      <c r="F48" s="106" t="e">
+      <c r="E48" s="128">
+        <v>150</v>
+      </c>
+      <c r="F48" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G48" s="106" t="e">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="G48" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="129">
         <v>48</v>
       </c>
-      <c r="B49" s="128"/>
+      <c r="B49" s="128" t="s">
+        <v>818</v>
+      </c>
       <c r="C49" s="128"/>
       <c r="D49" s="128"/>
-      <c r="E49" s="128"/>
-      <c r="F49" s="106" t="e">
+      <c r="E49" s="128">
+        <v>36</v>
+      </c>
+      <c r="F49" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G49" s="106" t="e">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="G49" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="129">
         <v>49</v>
       </c>
-      <c r="B50" s="128"/>
+      <c r="B50" s="128" t="s">
+        <v>819</v>
+      </c>
       <c r="C50" s="128"/>
       <c r="D50" s="128"/>
-      <c r="E50" s="128"/>
-      <c r="F50" s="106" t="e">
+      <c r="E50" s="128">
+        <v>95</v>
+      </c>
+      <c r="F50" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G50" s="106" t="e">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="G50" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.42105263157894735</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="129">
         <v>50</v>
       </c>
-      <c r="B51" s="128"/>
+      <c r="B51" s="128" t="s">
+        <v>820</v>
+      </c>
       <c r="C51" s="128"/>
       <c r="D51" s="128"/>
-      <c r="E51" s="128"/>
-      <c r="F51" s="106" t="e">
+      <c r="E51" s="128">
+        <v>36</v>
+      </c>
+      <c r="F51" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G51" s="106" t="e">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="G51" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="129">
         <v>51</v>
       </c>
-      <c r="B52" s="128"/>
+      <c r="B52" s="128" t="s">
+        <v>821</v>
+      </c>
       <c r="C52" s="128"/>
       <c r="D52" s="128"/>
-      <c r="E52" s="128"/>
-      <c r="F52" s="106" t="e">
+      <c r="E52" s="128">
+        <v>95</v>
+      </c>
+      <c r="F52" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G52" s="106" t="e">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="G52" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.42105263157894735</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="129">
         <v>52</v>
       </c>
-      <c r="B53" s="128"/>
+      <c r="B53" s="128" t="s">
+        <v>822</v>
+      </c>
       <c r="C53" s="128"/>
       <c r="D53" s="128"/>
-      <c r="E53" s="128"/>
-      <c r="F53" s="106" t="e">
+      <c r="E53" s="128">
+        <v>5</v>
+      </c>
+      <c r="F53" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G53" s="106" t="e">
+        <v>8</v>
+      </c>
+      <c r="G53" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="129">
         <v>53</v>
       </c>
-      <c r="B54" s="128"/>
+      <c r="B54" s="128" t="s">
+        <v>823</v>
+      </c>
       <c r="C54" s="128"/>
       <c r="D54" s="128"/>
-      <c r="E54" s="128"/>
-      <c r="F54" s="106" t="e">
+      <c r="E54" s="128">
+        <v>1.3</v>
+      </c>
+      <c r="F54" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G54" s="106" t="e">
+        <v>30.769230769230766</v>
+      </c>
+      <c r="G54" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>30.769230769230766</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="129">
         <v>54</v>
       </c>
-      <c r="B55" s="128"/>
+      <c r="B55" s="128" t="s">
+        <v>824</v>
+      </c>
       <c r="C55" s="128"/>
       <c r="D55" s="128"/>
-      <c r="E55" s="128"/>
-      <c r="F55" s="106" t="e">
+      <c r="E55" s="128">
+        <v>90</v>
+      </c>
+      <c r="F55" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G55" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G55" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="129">
         <v>55</v>
       </c>
-      <c r="B56" s="128"/>
+      <c r="B56" s="128" t="s">
+        <v>825</v>
+      </c>
       <c r="C56" s="128"/>
       <c r="D56" s="128"/>
-      <c r="E56" s="128"/>
-      <c r="F56" s="106" t="e">
+      <c r="E56" s="128">
+        <v>40</v>
+      </c>
+      <c r="F56" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G56" s="106" t="e">
+        <v>1</v>
+      </c>
+      <c r="G56" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="129">
         <v>56</v>
       </c>
-      <c r="B57" s="128"/>
+      <c r="B57" s="128" t="s">
+        <v>826</v>
+      </c>
       <c r="C57" s="128"/>
       <c r="D57" s="128"/>
-      <c r="E57" s="128"/>
-      <c r="F57" s="106" t="e">
+      <c r="E57" s="128">
+        <v>9</v>
+      </c>
+      <c r="F57" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G57" s="106" t="e">
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="G57" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="129">
         <v>57</v>
       </c>
-      <c r="B58" s="128"/>
+      <c r="B58" s="128" t="s">
+        <v>827</v>
+      </c>
       <c r="C58" s="128"/>
       <c r="D58" s="128"/>
-      <c r="E58" s="128"/>
-      <c r="F58" s="106" t="e">
+      <c r="E58" s="128">
+        <v>3</v>
+      </c>
+      <c r="F58" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G58" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G58" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="129">
         <v>58</v>
       </c>
-      <c r="B59" s="128"/>
+      <c r="B59" s="128" t="s">
+        <v>828</v>
+      </c>
       <c r="C59" s="128"/>
       <c r="D59" s="128"/>
-      <c r="E59" s="128"/>
-      <c r="F59" s="106" t="e">
+      <c r="E59" s="128">
+        <v>90</v>
+      </c>
+      <c r="F59" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G59" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G59" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="129">
         <v>59</v>
       </c>
-      <c r="B60" s="128"/>
+      <c r="B60" s="128" t="s">
+        <v>829</v>
+      </c>
       <c r="C60" s="128"/>
       <c r="D60" s="128"/>
-      <c r="E60" s="128"/>
-      <c r="F60" s="106" t="e">
+      <c r="E60" s="128">
+        <v>3</v>
+      </c>
+      <c r="F60" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G60" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G60" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="129">
         <v>60</v>
       </c>
-      <c r="B61" s="128"/>
+      <c r="B61" s="128" t="s">
+        <v>830</v>
+      </c>
       <c r="C61" s="128"/>
       <c r="D61" s="128"/>
-      <c r="E61" s="128"/>
-      <c r="F61" s="106" t="e">
+      <c r="E61" s="128">
+        <v>1.3</v>
+      </c>
+      <c r="F61" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G61" s="106" t="e">
+        <v>30.769230769230766</v>
+      </c>
+      <c r="G61" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>30.769230769230766</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="129">
         <v>61</v>
       </c>
-      <c r="B62" s="128"/>
+      <c r="B62" s="128" t="s">
+        <v>831</v>
+      </c>
       <c r="C62" s="128"/>
       <c r="D62" s="128"/>
-      <c r="E62" s="128"/>
-      <c r="F62" s="106" t="e">
+      <c r="E62" s="128">
+        <v>90</v>
+      </c>
+      <c r="F62" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G62" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G62" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="129">
         <v>62</v>
       </c>
-      <c r="B63" s="128"/>
+      <c r="B63" s="128" t="s">
+        <v>832</v>
+      </c>
       <c r="C63" s="128"/>
       <c r="D63" s="128"/>
-      <c r="E63" s="128"/>
-      <c r="F63" s="106" t="e">
+      <c r="E63" s="128">
+        <v>40</v>
+      </c>
+      <c r="F63" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G63" s="106" t="e">
+        <v>1</v>
+      </c>
+      <c r="G63" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="129">
         <v>63</v>
       </c>
-      <c r="B64" s="128"/>
+      <c r="B64" s="128" t="s">
+        <v>833</v>
+      </c>
       <c r="C64" s="128"/>
       <c r="D64" s="128"/>
-      <c r="E64" s="128"/>
-      <c r="F64" s="106" t="e">
+      <c r="E64" s="128">
+        <v>9</v>
+      </c>
+      <c r="F64" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G64" s="106" t="e">
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="G64" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="129">
         <v>64</v>
       </c>
-      <c r="B65" s="128"/>
+      <c r="B65" s="128" t="s">
+        <v>834</v>
+      </c>
       <c r="C65" s="128"/>
       <c r="D65" s="128"/>
-      <c r="E65" s="128"/>
-      <c r="F65" s="106" t="e">
+      <c r="E65" s="128">
+        <v>3</v>
+      </c>
+      <c r="F65" s="106">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G65" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G65" s="106">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="129">
         <v>65</v>
       </c>
-      <c r="B66" s="128"/>
+      <c r="B66" s="128" t="s">
+        <v>835</v>
+      </c>
       <c r="C66" s="128"/>
       <c r="D66" s="128"/>
-      <c r="E66" s="128"/>
-      <c r="F66" s="106" t="e">
+      <c r="E66" s="128">
+        <v>90</v>
+      </c>
+      <c r="F66" s="106">
         <f t="shared" ref="F66:F97" si="4">40/E66</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G66" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G66" s="106">
         <f t="shared" ref="G66:G97" si="5">IF(E66&lt;0,150,F66)</f>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="129">
         <v>66</v>
       </c>
-      <c r="B67" s="128"/>
+      <c r="B67" s="128" t="s">
+        <v>836</v>
+      </c>
       <c r="C67" s="128"/>
       <c r="D67" s="128"/>
-      <c r="E67" s="128"/>
-      <c r="F67" s="106" t="e">
+      <c r="E67" s="128">
+        <v>3</v>
+      </c>
+      <c r="F67" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G67" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G67" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="129">
         <v>67</v>
       </c>
-      <c r="B68" s="128"/>
+      <c r="B68" s="128" t="s">
+        <v>837</v>
+      </c>
       <c r="C68" s="128"/>
       <c r="D68" s="128"/>
-      <c r="E68" s="128"/>
-      <c r="F68" s="106" t="e">
+      <c r="E68" s="128">
+        <v>36</v>
+      </c>
+      <c r="F68" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G68" s="106" t="e">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="G68" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="129">
         <v>68</v>
       </c>
-      <c r="B69" s="128"/>
+      <c r="B69" s="128" t="s">
+        <v>838</v>
+      </c>
       <c r="C69" s="128"/>
       <c r="D69" s="128"/>
-      <c r="E69" s="128"/>
-      <c r="F69" s="106" t="e">
+      <c r="E69" s="128">
+        <v>95</v>
+      </c>
+      <c r="F69" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G69" s="106" t="e">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="G69" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.42105263157894735</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="129">
         <v>69</v>
       </c>
-      <c r="B70" s="128"/>
+      <c r="B70" s="128" t="s">
+        <v>839</v>
+      </c>
       <c r="C70" s="128"/>
       <c r="D70" s="128"/>
-      <c r="E70" s="128"/>
-      <c r="F70" s="106" t="e">
+      <c r="E70" s="128">
+        <v>36</v>
+      </c>
+      <c r="F70" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G70" s="106" t="e">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="G70" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="129">
         <v>70</v>
       </c>
-      <c r="B71" s="128"/>
+      <c r="B71" s="128" t="s">
+        <v>840</v>
+      </c>
       <c r="C71" s="128"/>
       <c r="D71" s="128"/>
-      <c r="E71" s="128"/>
-      <c r="F71" s="106" t="e">
+      <c r="E71" s="128">
+        <v>95</v>
+      </c>
+      <c r="F71" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G71" s="106" t="e">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="G71" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.42105263157894735</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="129">
         <v>71</v>
       </c>
-      <c r="B72" s="128"/>
+      <c r="B72" s="128" t="s">
+        <v>841</v>
+      </c>
       <c r="C72" s="128"/>
       <c r="D72" s="128"/>
-      <c r="E72" s="128"/>
-      <c r="F72" s="106" t="e">
+      <c r="E72" s="128">
+        <v>5</v>
+      </c>
+      <c r="F72" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G72" s="106" t="e">
+        <v>8</v>
+      </c>
+      <c r="G72" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="129">
         <v>72</v>
       </c>
-      <c r="B73" s="128"/>
+      <c r="B73" s="128" t="s">
+        <v>842</v>
+      </c>
       <c r="C73" s="128"/>
       <c r="D73" s="128"/>
-      <c r="E73" s="128"/>
-      <c r="F73" s="106" t="e">
+      <c r="E73" s="128">
+        <v>3</v>
+      </c>
+      <c r="F73" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G73" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G73" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="129">
         <v>73</v>
       </c>
-      <c r="B74" s="128"/>
+      <c r="B74" s="128" t="s">
+        <v>843</v>
+      </c>
       <c r="C74" s="128"/>
       <c r="D74" s="128"/>
-      <c r="E74" s="128"/>
-      <c r="F74" s="106" t="e">
+      <c r="E74" s="128">
+        <v>90</v>
+      </c>
+      <c r="F74" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G74" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G74" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="129">
         <v>74</v>
       </c>
-      <c r="B75" s="128"/>
+      <c r="B75" s="128" t="s">
+        <v>844</v>
+      </c>
       <c r="C75" s="128"/>
       <c r="D75" s="128"/>
-      <c r="E75" s="128"/>
-      <c r="F75" s="106" t="e">
+      <c r="E75" s="128">
+        <v>3</v>
+      </c>
+      <c r="F75" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G75" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G75" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="129">
         <v>75</v>
       </c>
-      <c r="B76" s="128"/>
+      <c r="B76" s="128" t="s">
+        <v>845</v>
+      </c>
       <c r="C76" s="128"/>
       <c r="D76" s="128"/>
-      <c r="E76" s="128"/>
-      <c r="F76" s="106" t="e">
+      <c r="E76" s="128">
+        <v>50</v>
+      </c>
+      <c r="F76" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G76" s="106" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="G76" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="129">
         <v>76</v>
       </c>
-      <c r="B77" s="128"/>
+      <c r="B77" s="128" t="s">
+        <v>846</v>
+      </c>
       <c r="C77" s="128"/>
       <c r="D77" s="128"/>
-      <c r="E77" s="128"/>
-      <c r="F77" s="106" t="e">
+      <c r="E77" s="128">
+        <v>150</v>
+      </c>
+      <c r="F77" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G77" s="106" t="e">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="G77" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="129">
         <v>77</v>
       </c>
-      <c r="B78" s="128"/>
+      <c r="B78" s="128" t="s">
+        <v>847</v>
+      </c>
       <c r="C78" s="128"/>
       <c r="D78" s="128"/>
-      <c r="E78" s="128"/>
-      <c r="F78" s="106" t="e">
+      <c r="E78" s="128">
+        <v>36</v>
+      </c>
+      <c r="F78" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G78" s="106" t="e">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="G78" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="129">
         <v>78</v>
       </c>
-      <c r="B79" s="128"/>
+      <c r="B79" s="128" t="s">
+        <v>848</v>
+      </c>
       <c r="C79" s="128"/>
       <c r="D79" s="128"/>
-      <c r="E79" s="128"/>
-      <c r="F79" s="106" t="e">
+      <c r="E79" s="128">
+        <v>95</v>
+      </c>
+      <c r="F79" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G79" s="106" t="e">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="G79" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.42105263157894735</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="129">
         <v>79</v>
       </c>
-      <c r="B80" s="128"/>
+      <c r="B80" s="128" t="s">
+        <v>849</v>
+      </c>
       <c r="C80" s="128"/>
       <c r="D80" s="128"/>
-      <c r="E80" s="128"/>
-      <c r="F80" s="106" t="e">
+      <c r="E80" s="128">
+        <v>36</v>
+      </c>
+      <c r="F80" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G80" s="106" t="e">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="G80" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="129">
         <v>80</v>
       </c>
-      <c r="B81" s="128"/>
+      <c r="B81" s="128" t="s">
+        <v>850</v>
+      </c>
       <c r="C81" s="128"/>
       <c r="D81" s="128"/>
-      <c r="E81" s="128"/>
-      <c r="F81" s="106" t="e">
+      <c r="E81" s="128">
+        <v>95</v>
+      </c>
+      <c r="F81" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G81" s="106" t="e">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="G81" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.42105263157894735</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="129">
         <v>81</v>
       </c>
-      <c r="B82" s="128"/>
+      <c r="B82" s="128" t="s">
+        <v>851</v>
+      </c>
       <c r="C82" s="128"/>
       <c r="D82" s="128"/>
-      <c r="E82" s="128"/>
-      <c r="F82" s="106" t="e">
+      <c r="E82" s="128">
+        <v>5</v>
+      </c>
+      <c r="F82" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G82" s="106" t="e">
+        <v>8</v>
+      </c>
+      <c r="G82" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="129">
         <v>82</v>
       </c>
-      <c r="B83" s="128"/>
+      <c r="B83" s="128" t="s">
+        <v>852</v>
+      </c>
       <c r="C83" s="128"/>
       <c r="D83" s="128"/>
-      <c r="E83" s="128"/>
-      <c r="F83" s="106" t="e">
+      <c r="E83" s="128">
+        <v>1.3</v>
+      </c>
+      <c r="F83" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G83" s="106" t="e">
+        <v>30.769230769230766</v>
+      </c>
+      <c r="G83" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>30.769230769230766</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="129">
         <v>83</v>
       </c>
-      <c r="B84" s="128"/>
+      <c r="B84" s="128" t="s">
+        <v>853</v>
+      </c>
       <c r="C84" s="128"/>
       <c r="D84" s="128"/>
-      <c r="E84" s="128"/>
-      <c r="F84" s="106" t="e">
+      <c r="E84" s="128">
+        <v>90</v>
+      </c>
+      <c r="F84" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G84" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G84" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="129">
         <v>84</v>
       </c>
-      <c r="B85" s="128"/>
+      <c r="B85" s="128" t="s">
+        <v>854</v>
+      </c>
       <c r="C85" s="128"/>
       <c r="D85" s="128"/>
-      <c r="E85" s="128"/>
-      <c r="F85" s="106" t="e">
+      <c r="E85" s="128">
+        <v>40</v>
+      </c>
+      <c r="F85" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G85" s="106" t="e">
+        <v>1</v>
+      </c>
+      <c r="G85" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="129">
         <v>85</v>
       </c>
-      <c r="B86" s="128"/>
+      <c r="B86" s="128" t="s">
+        <v>855</v>
+      </c>
       <c r="C86" s="128"/>
       <c r="D86" s="128"/>
-      <c r="E86" s="128"/>
-      <c r="F86" s="106" t="e">
+      <c r="E86" s="128">
+        <v>9</v>
+      </c>
+      <c r="F86" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G86" s="106" t="e">
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="G86" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="129">
         <v>86</v>
       </c>
-      <c r="B87" s="128"/>
+      <c r="B87" s="128" t="s">
+        <v>856</v>
+      </c>
       <c r="C87" s="128"/>
       <c r="D87" s="128"/>
-      <c r="E87" s="128"/>
-      <c r="F87" s="106" t="e">
+      <c r="E87" s="128">
+        <v>3</v>
+      </c>
+      <c r="F87" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G87" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G87" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="129">
         <v>87</v>
       </c>
-      <c r="B88" s="128"/>
+      <c r="B88" s="128" t="s">
+        <v>857</v>
+      </c>
       <c r="C88" s="128"/>
       <c r="D88" s="128"/>
-      <c r="E88" s="128"/>
-      <c r="F88" s="106" t="e">
+      <c r="E88" s="128">
+        <v>90</v>
+      </c>
+      <c r="F88" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G88" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G88" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="129">
         <v>88</v>
       </c>
-      <c r="B89" s="128"/>
+      <c r="B89" s="128" t="s">
+        <v>858</v>
+      </c>
       <c r="C89" s="128"/>
       <c r="D89" s="128"/>
-      <c r="E89" s="128"/>
-      <c r="F89" s="106" t="e">
+      <c r="E89" s="128">
+        <v>3</v>
+      </c>
+      <c r="F89" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G89" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G89" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="129">
         <v>89</v>
       </c>
-      <c r="B90" s="128"/>
+      <c r="B90" s="128" t="s">
+        <v>859</v>
+      </c>
       <c r="C90" s="128"/>
       <c r="D90" s="128"/>
-      <c r="E90" s="128"/>
-      <c r="F90" s="106" t="e">
+      <c r="E90" s="128">
+        <v>1.3</v>
+      </c>
+      <c r="F90" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G90" s="106" t="e">
+        <v>30.769230769230766</v>
+      </c>
+      <c r="G90" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>30.769230769230766</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="129">
         <v>90</v>
       </c>
-      <c r="B91" s="128"/>
+      <c r="B91" s="128" t="s">
+        <v>860</v>
+      </c>
       <c r="C91" s="128"/>
       <c r="D91" s="128"/>
-      <c r="E91" s="128"/>
-      <c r="F91" s="106" t="e">
+      <c r="E91" s="128">
+        <v>90</v>
+      </c>
+      <c r="F91" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G91" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G91" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="129">
         <v>91</v>
       </c>
-      <c r="B92" s="128"/>
+      <c r="B92" s="128" t="s">
+        <v>861</v>
+      </c>
       <c r="C92" s="128"/>
       <c r="D92" s="128"/>
-      <c r="E92" s="128"/>
-      <c r="F92" s="106" t="e">
+      <c r="E92" s="128">
+        <v>40</v>
+      </c>
+      <c r="F92" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G92" s="106" t="e">
+        <v>1</v>
+      </c>
+      <c r="G92" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="129">
         <v>92</v>
       </c>
-      <c r="B93" s="128"/>
+      <c r="B93" s="128" t="s">
+        <v>862</v>
+      </c>
       <c r="C93" s="128"/>
       <c r="D93" s="128"/>
-      <c r="E93" s="128"/>
-      <c r="F93" s="106" t="e">
+      <c r="E93" s="128">
+        <v>9</v>
+      </c>
+      <c r="F93" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G93" s="106" t="e">
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="G93" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="129">
         <v>93</v>
       </c>
-      <c r="B94" s="128"/>
+      <c r="B94" s="128" t="s">
+        <v>863</v>
+      </c>
       <c r="C94" s="128"/>
       <c r="D94" s="128"/>
-      <c r="E94" s="128"/>
-      <c r="F94" s="106" t="e">
+      <c r="E94" s="128">
+        <v>3</v>
+      </c>
+      <c r="F94" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G94" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G94" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="129">
         <v>94</v>
       </c>
-      <c r="B95" s="128"/>
+      <c r="B95" s="128" t="s">
+        <v>864</v>
+      </c>
       <c r="C95" s="128"/>
       <c r="D95" s="128"/>
-      <c r="E95" s="128"/>
-      <c r="F95" s="106" t="e">
+      <c r="E95" s="128">
+        <v>90</v>
+      </c>
+      <c r="F95" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G95" s="106" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G95" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="129">
         <v>95</v>
       </c>
-      <c r="B96" s="128"/>
+      <c r="B96" s="128" t="s">
+        <v>865</v>
+      </c>
       <c r="C96" s="128"/>
       <c r="D96" s="128"/>
-      <c r="E96" s="128"/>
-      <c r="F96" s="106" t="e">
+      <c r="E96" s="128">
+        <v>3</v>
+      </c>
+      <c r="F96" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G96" s="106" t="e">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G96" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="129">
         <v>96</v>
       </c>
-      <c r="B97" s="128"/>
+      <c r="B97" s="128" t="s">
+        <v>866</v>
+      </c>
       <c r="C97" s="128"/>
       <c r="D97" s="128"/>
-      <c r="E97" s="128"/>
-      <c r="F97" s="106" t="e">
+      <c r="E97" s="128">
+        <v>36</v>
+      </c>
+      <c r="F97" s="106">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G97" s="106" t="e">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="G97" s="106">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>